<commit_message>
fix bug for room capacity
</commit_message>
<xml_diff>
--- a/data/Input/ClassRoom.xlsx
+++ b/data/Input/ClassRoom.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7E36E6B0-C95F-224F-83AD-EEB11BAC00E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A30F702-BA93-E344-8684-87DFD54529CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="3160" windowWidth="27240" windowHeight="16440"/>
+    <workbookView xWindow="-420" yWindow="3120" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="room" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="53">
   <si>
     <t>RoomID</t>
   </si>
@@ -140,13 +140,52 @@
   </si>
   <si>
     <t>·</t>
+  </si>
+  <si>
+    <t>Genome Science G100 (426 seats)</t>
+  </si>
+  <si>
+    <t>Hamilton 100 (403 seats)</t>
+  </si>
+  <si>
+    <t>Stone Center 103 (353 seats)</t>
+  </si>
+  <si>
+    <t>Hanes Art Center 121 (296 seats)</t>
+  </si>
+  <si>
+    <t>Global Education Center 1015 (246 seats)</t>
+  </si>
+  <si>
+    <t>Genome Science G200 (237 seats)</t>
+  </si>
+  <si>
+    <t>Chapman 211 (224 seats)</t>
+  </si>
+  <si>
+    <t>Carroll 111 (210 seats)</t>
+  </si>
+  <si>
+    <t>Murray G202 (209 seats)</t>
+  </si>
+  <si>
+    <t>Coker 201 (198 seats)</t>
+  </si>
+  <si>
+    <t>Manning 209 (188 seats)</t>
+  </si>
+  <si>
+    <t>Chapman 201 (186 seats)</t>
+  </si>
+  <si>
+    <t>TTH_2,3,4,5,6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -277,6 +316,26 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF007FAE"/>
+      <name val="Open Sans"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -579,7 +638,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -622,11 +681,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -660,6 +723,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -979,14 +1043,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D33" sqref="A16:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.83203125" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1453,7 +1522,178 @@
         <v>6</v>
       </c>
     </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="3">
+        <v>426</v>
+      </c>
+      <c r="D34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="3">
+        <v>403</v>
+      </c>
+      <c r="D35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="3">
+        <v>353</v>
+      </c>
+      <c r="D36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="3">
+        <v>296</v>
+      </c>
+      <c r="D37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="3">
+        <v>246</v>
+      </c>
+      <c r="D38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="3">
+        <v>237</v>
+      </c>
+      <c r="D39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="3">
+        <v>224</v>
+      </c>
+      <c r="D40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="3">
+        <v>210</v>
+      </c>
+      <c r="D41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="3">
+        <v>209</v>
+      </c>
+      <c r="D42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" s="3">
+        <v>198</v>
+      </c>
+      <c r="D43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="3">
+        <v>188</v>
+      </c>
+      <c r="D44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="3">
+        <v>186</v>
+      </c>
+      <c r="D45" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A34" r:id="rId1" display="https://hotline.unc.edu/public/?classroom3&amp;room=Genome%20Science%20G100" xr:uid="{CC73FE38-312B-2D48-9424-A9FD126DEEAC}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove the 0 preference for facultys
</commit_message>
<xml_diff>
--- a/data/Input/ClassRoom.xlsx
+++ b/data/Input/ClassRoom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A30F702-BA93-E344-8684-87DFD54529CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C65CF79-A658-874E-BA74-77AEEEB1D668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-420" yWindow="3120" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="54">
   <si>
     <t>RoomID</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>TTH_2,3,4,5,6</t>
+  </si>
+  <si>
+    <t>TTH_2,3;MW_1,2,3,4,5,6,7</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1050,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D33" sqref="A16:D33"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1533,7 +1536,7 @@
         <v>426</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1575,7 +1578,7 @@
         <v>296</v>
       </c>
       <c r="D37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1589,7 +1592,7 @@
         <v>246</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix priority room by CS, campus, backup
</commit_message>
<xml_diff>
--- a/data/Input/ClassRoom.xlsx
+++ b/data/Input/ClassRoom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C65CF79-A658-874E-BA74-77AEEEB1D668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F5E92E-6BA4-6F42-AC84-D511DED82B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-420" yWindow="3120" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3120" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="room" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="55">
   <si>
     <t>RoomID</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>TTH_2,3;MW_1,2,3,4,5,6,7</t>
+  </si>
+  <si>
+    <t>backup</t>
   </si>
 </sst>
 </file>
@@ -1049,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1275,7 +1278,7 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C16">
         <v>200</v>
@@ -1289,7 +1292,7 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C17">
         <v>200</v>
@@ -1303,7 +1306,7 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C18">
         <v>200</v>
@@ -1317,7 +1320,7 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C19">
         <v>200</v>
@@ -1331,7 +1334,7 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C20">
         <v>200</v>
@@ -1345,7 +1348,7 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C21">
         <v>200</v>
@@ -1359,7 +1362,7 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C22">
         <v>250</v>
@@ -1373,7 +1376,7 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C23">
         <v>250</v>
@@ -1387,7 +1390,7 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C24">
         <v>250</v>
@@ -1401,7 +1404,7 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C25">
         <v>250</v>
@@ -1415,7 +1418,7 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C26">
         <v>250</v>
@@ -1429,7 +1432,7 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C27">
         <v>250</v>
@@ -1443,7 +1446,7 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C28">
         <v>300</v>
@@ -1457,7 +1460,7 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C29">
         <v>300</v>
@@ -1471,7 +1474,7 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C30">
         <v>300</v>
@@ -1488,7 +1491,7 @@
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C31">
         <v>300</v>
@@ -1502,7 +1505,7 @@
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C32">
         <v>300</v>
@@ -1516,7 +1519,7 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C33">
         <v>300</v>

</xml_diff>

<commit_message>
New feature: Some faculty can be scheduled in specific time slot and room
</commit_message>
<xml_diff>
--- a/data/Input/ClassRoom.xlsx
+++ b/data/Input/ClassRoom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minyuamzhang/Documents/UNC/2025 Spring/COMP 523/UNC-CS-Course-Scheduling-mk2/data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F5E92E-6BA4-6F42-AC84-D511DED82B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEEEAEF-A9CC-A945-AF20-0F7BFCD553E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="3120" windowWidth="27240" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="58">
   <si>
     <t>RoomID</t>
   </si>
@@ -185,13 +185,22 @@
   </si>
   <si>
     <t>backup</t>
+  </si>
+  <si>
+    <t>TTH_2</t>
+  </si>
+  <si>
+    <t>MWF_8,9;TTH_7</t>
+  </si>
+  <si>
+    <t>Greenlaw Hall-Rm 0101 (100 seats)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -345,6 +354,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -689,11 +704,12 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1050,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1628,13 +1644,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B41" t="s">
         <v>21</v>
       </c>
       <c r="C41" s="3">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D41" t="s">
         <v>52</v>
@@ -1642,13 +1658,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B42" t="s">
         <v>21</v>
       </c>
       <c r="C42" s="3">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D42" t="s">
         <v>52</v>
@@ -1656,13 +1672,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B43" t="s">
         <v>21</v>
       </c>
       <c r="C43" s="3">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="D43" t="s">
         <v>52</v>
@@ -1670,30 +1686,44 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B44" t="s">
         <v>21</v>
       </c>
       <c r="C44" s="3">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D44" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>51</v>
+    <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="B45" t="s">
         <v>21</v>
       </c>
       <c r="C45" s="3">
-        <v>186</v>
+        <v>100</v>
       </c>
       <c r="D45" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="3">
+        <v>210</v>
+      </c>
+      <c r="D46" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>